<commit_message>
Pu example for Dawn and pressure-depth tweaks.
</commit_message>
<xml_diff>
--- a/Benchmarking/liquid, olivine/PythonInput_OlLiq_Thermometers_Putirka.xlsx
+++ b/Benchmarking/liquid, olivine/PythonInput_OlLiq_Thermometers_Putirka.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Benchmarking\liquid, olivine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Postdoc\MyBarometers\Thermobar_outer\Benchmarking\liquid, olivine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF38EE97-0640-4880-ADA4-2B544994A110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A00B09-2BD3-42AE-8465-660B9FE49436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{81A2371C-1752-7741-8A48-BEC2C378A224}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{81A2371C-1752-7741-8A48-BEC2C378A224}"/>
   </bookViews>
   <sheets>
     <sheet name="SM Tab4_editedMM" sheetId="4" r:id="rId1"/>
     <sheet name="Pu2017_2021_NiThermometers" sheetId="5" r:id="rId2"/>
-    <sheet name="SM Tab4" sheetId="1" r:id="rId3"/>
-    <sheet name="Error_Example_Abs" sheetId="2" r:id="rId4"/>
-    <sheet name="Error_Example_Perc" sheetId="3" r:id="rId5"/>
+    <sheet name="T_Pu2017_iteration" sheetId="6" r:id="rId3"/>
+    <sheet name="SM Tab4" sheetId="1" r:id="rId4"/>
+    <sheet name="Error_Example_Abs" sheetId="2" r:id="rId5"/>
+    <sheet name="Error_Example_Perc" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -136,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="122">
   <si>
     <t>P_GPa</t>
   </si>
@@ -364,6 +365,144 @@
   </si>
   <si>
     <t>Temp_2017Calculator</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>22CLDB140</t>
+  </si>
+  <si>
+    <t>20CLDB001a</t>
+  </si>
+  <si>
+    <t>CLDR013</t>
+  </si>
+  <si>
+    <t>20CLDB013</t>
+  </si>
+  <si>
+    <t>21CLDB058</t>
+  </si>
+  <si>
+    <t>22CLDB108</t>
+  </si>
+  <si>
+    <t>20CLDB009</t>
+  </si>
+  <si>
+    <t>20CLDB014</t>
+  </si>
+  <si>
+    <t>20CLDB019</t>
+  </si>
+  <si>
+    <t>21CLDB047</t>
+  </si>
+  <si>
+    <t>21CLDB084</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Cr2O3</t>
+  </si>
+  <si>
+    <t>Fo#</t>
+  </si>
+  <si>
+    <t>olvcore1</t>
+  </si>
+  <si>
+    <t>olvcore9</t>
+  </si>
+  <si>
+    <t>olvccore10</t>
+  </si>
+  <si>
+    <t>olvcore8</t>
+  </si>
+  <si>
+    <t>olvcore6</t>
+  </si>
+  <si>
+    <t>olvcore4</t>
+  </si>
+  <si>
+    <t>olvcore3_1</t>
+  </si>
+  <si>
+    <t>olvcore10_3</t>
+  </si>
+  <si>
+    <t>olvcore9_3</t>
+  </si>
+  <si>
+    <t>olvcore7_3</t>
+  </si>
+  <si>
+    <t>olvxeno1_4</t>
+  </si>
+  <si>
+    <t>olvcore6_5</t>
+  </si>
+  <si>
+    <t>olvcore7_1</t>
+  </si>
+  <si>
+    <t>olvcore2_1</t>
+  </si>
+  <si>
+    <t>olvcore5_ave</t>
+  </si>
+  <si>
+    <t>olvtr5_9</t>
+  </si>
+  <si>
+    <t>olvcore3_ave</t>
+  </si>
+  <si>
+    <t>olvcore6_1</t>
+  </si>
+  <si>
+    <t>olvcore8_ave</t>
+  </si>
+  <si>
+    <t>olvcore4_ave</t>
+  </si>
+  <si>
+    <t>olvxen6_ave</t>
+  </si>
+  <si>
+    <t>olvcore1_ave</t>
+  </si>
+  <si>
+    <t>olvcore11_ave</t>
+  </si>
+  <si>
+    <t>olvcore2_ave</t>
+  </si>
+  <si>
+    <t>TMg(˚C)</t>
+  </si>
+  <si>
+    <t>TNi(˚C)</t>
+  </si>
+  <si>
+    <t>∆T(˚C)</t>
+  </si>
+  <si>
+    <t>minH2O(wt%)</t>
+  </si>
+  <si>
+    <t>sample#</t>
+  </si>
+  <si>
+    <t>CoO</t>
+  </si>
+  <si>
+    <t>Ni(ppm)</t>
   </si>
 </sst>
 </file>
@@ -430,7 +569,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,8 +594,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF96C6FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -491,12 +636,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -548,6 +730,21 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,9 +770,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -613,7 +810,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -719,7 +916,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -861,7 +1058,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -914,23 +1111,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93241BA4-AD6A-476B-89F9-77C94F1FACB0}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="AA1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.296875" customWidth="1"/>
-    <col min="18" max="18" width="49.296875" customWidth="1"/>
-    <col min="29" max="33" width="11.19921875" style="6"/>
-    <col min="34" max="34" width="11.19921875" style="16" customWidth="1"/>
-    <col min="35" max="35" width="11.19921875" style="6"/>
-    <col min="36" max="37" width="11.19921875" style="6" customWidth="1"/>
-    <col min="43" max="43" width="11.19921875" style="20"/>
-    <col min="44" max="44" width="11.19921875" style="6"/>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="18" max="18" width="49.33203125" customWidth="1"/>
+    <col min="29" max="33" width="11.1640625" style="6"/>
+    <col min="34" max="34" width="11.1640625" style="16" customWidth="1"/>
+    <col min="35" max="35" width="11.1640625" style="6"/>
+    <col min="36" max="37" width="11.1640625" style="6" customWidth="1"/>
+    <col min="43" max="43" width="11.1640625" style="20"/>
+    <col min="44" max="44" width="11.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="13" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="13" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -1070,7 +1267,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1208,7 +1405,7 @@
         <v>1021.4979696584832</v>
       </c>
     </row>
-    <row r="3" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1346,7 +1543,7 @@
         <v>969.30498574021021</v>
       </c>
     </row>
-    <row r="4" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1484,7 +1681,7 @@
         <v>1008.3930249020459</v>
       </c>
     </row>
-    <row r="5" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1622,7 +1819,7 @@
         <v>932.40701771358897</v>
       </c>
     </row>
-    <row r="6" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1760,7 +1957,7 @@
         <v>994.52331680458246</v>
       </c>
     </row>
-    <row r="7" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1898,7 +2095,7 @@
         <v>980.59621209897716</v>
       </c>
     </row>
-    <row r="8" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2036,7 +2233,7 @@
         <v>970.9528707859962</v>
       </c>
     </row>
-    <row r="9" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2174,7 +2371,7 @@
         <v>938.81458266078494</v>
       </c>
     </row>
-    <row r="10" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -2312,7 +2509,7 @@
         <v>908.55701429787223</v>
       </c>
     </row>
-    <row r="11" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2450,7 +2647,7 @@
         <v>1046.2136650074403</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="P12" s="1"/>
     </row>
   </sheetData>
@@ -2464,12 +2661,12 @@
   <dimension ref="A1:AM6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:39" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" s="13" customFormat="1" ht="55" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -2558,7 +2755,7 @@
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
-    <row r="2" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2647,7 +2844,7 @@
       <c r="AG2" s="5"/>
       <c r="AM2" s="2"/>
     </row>
-    <row r="3" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2736,7 +2933,7 @@
       <c r="AG3" s="5"/>
       <c r="AM3" s="2"/>
     </row>
-    <row r="4" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2825,7 +3022,7 @@
       <c r="AG4" s="5"/>
       <c r="AM4" s="2"/>
     </row>
-    <row r="5" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2914,7 +3111,7 @@
       <c r="AG5" s="5"/>
       <c r="AM5" s="2"/>
     </row>
-    <row r="6" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -3010,6 +3207,3260 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE0ABF5-8F36-4DD1-882B-9813C1EBD20F}">
+  <dimension ref="A1:AE42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD1" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE1" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1263.6509312899279</v>
+      </c>
+      <c r="B2">
+        <v>1243.0513462721351</v>
+      </c>
+      <c r="C2">
+        <v>20.599585017792833</v>
+      </c>
+      <c r="D2">
+        <v>0.56803137115214342</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2">
+        <v>53.083518805267367</v>
+      </c>
+      <c r="G2">
+        <v>0.82599925119977946</v>
+      </c>
+      <c r="H2">
+        <v>13.734173947269662</v>
+      </c>
+      <c r="I2">
+        <v>8.1303299157904583</v>
+      </c>
+      <c r="J2">
+        <v>0.14681367119376357</v>
+      </c>
+      <c r="K2">
+        <v>11.156961421301775</v>
+      </c>
+      <c r="L2">
+        <v>8.8264035617834864</v>
+      </c>
+      <c r="M2">
+        <v>2.7967998231672899</v>
+      </c>
+      <c r="N2">
+        <v>1.1002383057751137</v>
+      </c>
+      <c r="O2">
+        <v>0.19876129725129035</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S2">
+        <v>330</v>
+      </c>
+      <c r="T2">
+        <f>10^(-4)*74.6928*S2/58.6934</f>
+        <v>4.1995563385321018E-2</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" s="22">
+        <v>41.24</v>
+      </c>
+      <c r="W2" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X2" s="22">
+        <v>7.77</v>
+      </c>
+      <c r="Y2" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="Z2" s="22">
+        <v>51.35</v>
+      </c>
+      <c r="AA2" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB2" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC2" s="24">
+        <v>0.49</v>
+      </c>
+      <c r="AD2" s="22">
+        <f>SUM(V2:AC2)</f>
+        <v>101.21</v>
+      </c>
+      <c r="AE2" s="26">
+        <f>(1/(1+1/(Z2/X2/(40.304/71.846))))*100</f>
+        <v>92.17574853036794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1266.2108404398086</v>
+      </c>
+      <c r="B3">
+        <v>1231.360166743746</v>
+      </c>
+      <c r="C3">
+        <v>34.850673696062586</v>
+      </c>
+      <c r="D3">
+        <v>0.99535810106698608</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3">
+        <v>53.083518805267367</v>
+      </c>
+      <c r="G3">
+        <v>0.82599925119977946</v>
+      </c>
+      <c r="H3">
+        <v>13.734173947269662</v>
+      </c>
+      <c r="I3">
+        <v>8.1303299157904583</v>
+      </c>
+      <c r="J3">
+        <v>0.14681367119376357</v>
+      </c>
+      <c r="K3">
+        <v>11.156961421301775</v>
+      </c>
+      <c r="L3">
+        <v>8.8264035617834864</v>
+      </c>
+      <c r="M3">
+        <v>2.7967998231672899</v>
+      </c>
+      <c r="N3">
+        <v>1.1002383057751137</v>
+      </c>
+      <c r="O3">
+        <v>0.19876129725129035</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S3">
+        <v>330</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T32" si="0">10^(-4)*74.6928*S3/58.6934</f>
+        <v>4.1995563385321018E-2</v>
+      </c>
+      <c r="U3" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="V3" s="22">
+        <v>40.950000000000003</v>
+      </c>
+      <c r="W3" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X3" s="22">
+        <v>8.32</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="Z3" s="22">
+        <v>50.56</v>
+      </c>
+      <c r="AA3" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="AB3" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="AC3" s="24">
+        <v>0.51</v>
+      </c>
+      <c r="AD3" s="22">
+        <f t="shared" ref="AD3:AD7" si="1">SUM(V3:AC3)</f>
+        <v>100.65</v>
+      </c>
+      <c r="AE3" s="26">
+        <f t="shared" ref="AE3:AE32" si="2">(1/(1+1/(Z3/X3/(40.304/71.846))))*100</f>
+        <v>91.548869590014874</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1265.4316751968313</v>
+      </c>
+      <c r="B4">
+        <v>1252.1712519487191</v>
+      </c>
+      <c r="C4">
+        <v>13.260423248112147</v>
+      </c>
+      <c r="D4">
+        <v>0.35892301528277565</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4">
+        <v>53.083518805267367</v>
+      </c>
+      <c r="G4">
+        <v>0.82599925119977946</v>
+      </c>
+      <c r="H4">
+        <v>13.734173947269662</v>
+      </c>
+      <c r="I4">
+        <v>8.1303299157904583</v>
+      </c>
+      <c r="J4">
+        <v>0.14681367119376357</v>
+      </c>
+      <c r="K4">
+        <v>11.156961421301775</v>
+      </c>
+      <c r="L4">
+        <v>8.8264035617834864</v>
+      </c>
+      <c r="M4">
+        <v>2.7967998231672899</v>
+      </c>
+      <c r="N4">
+        <v>1.1002383057751137</v>
+      </c>
+      <c r="O4">
+        <v>0.19876129725129035</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S4">
+        <v>330</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>4.1995563385321018E-2</v>
+      </c>
+      <c r="U4" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="V4" s="22">
+        <v>41.05</v>
+      </c>
+      <c r="W4" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="X4" s="22">
+        <v>8.24</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="Z4" s="22">
+        <v>50.86</v>
+      </c>
+      <c r="AA4" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="AB4" s="23">
+        <v>0.06</v>
+      </c>
+      <c r="AC4" s="24">
+        <v>0.47</v>
+      </c>
+      <c r="AD4" s="22">
+        <f t="shared" si="1"/>
+        <v>100.95000000000002</v>
+      </c>
+      <c r="AE4" s="26">
+        <f t="shared" si="2"/>
+        <v>91.668617149479772</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1254.5557699225328</v>
+      </c>
+      <c r="B5">
+        <v>1133.6619582822896</v>
+      </c>
+      <c r="C5">
+        <v>120.89381164024326</v>
+      </c>
+      <c r="D5">
+        <v>4.1723290378444045</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5">
+        <v>67.729723803163665</v>
+      </c>
+      <c r="G5">
+        <v>0.24200863177409873</v>
+      </c>
+      <c r="H5">
+        <v>14.719666689923949</v>
+      </c>
+      <c r="I5">
+        <v>2.5027161182931814</v>
+      </c>
+      <c r="J5">
+        <v>5.4920410258454865E-2</v>
+      </c>
+      <c r="K5">
+        <v>4.9851984012279855</v>
+      </c>
+      <c r="L5">
+        <v>2.8011402713128071</v>
+      </c>
+      <c r="M5">
+        <v>4.2805027559879196</v>
+      </c>
+      <c r="N5">
+        <v>2.5879374445563008</v>
+      </c>
+      <c r="O5">
+        <v>9.6185473501649618E-2</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>100.00000000000003</v>
+      </c>
+      <c r="S5">
+        <v>203</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>2.5833634446121714E-2</v>
+      </c>
+      <c r="U5" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="V5" s="22">
+        <v>41.11</v>
+      </c>
+      <c r="W5" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="X5" s="22">
+        <v>7.75</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="Z5" s="22">
+        <v>50.9</v>
+      </c>
+      <c r="AA5" s="23">
+        <v>0.06</v>
+      </c>
+      <c r="AB5" s="23">
+        <v>0.08</v>
+      </c>
+      <c r="AC5" s="24">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="AD5" s="22">
+        <f t="shared" si="1"/>
+        <v>101.17999999999999</v>
+      </c>
+      <c r="AE5" s="26">
+        <f t="shared" si="2"/>
+        <v>92.130737642698961</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1261.8816344200641</v>
+      </c>
+      <c r="B6">
+        <v>1145.7005990886328</v>
+      </c>
+      <c r="C6">
+        <v>116.1810353314313</v>
+      </c>
+      <c r="D6">
+        <v>3.9718065125320621</v>
+      </c>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6">
+        <v>67.729723803163665</v>
+      </c>
+      <c r="G6">
+        <v>0.24200863177409873</v>
+      </c>
+      <c r="H6">
+        <v>14.719666689923949</v>
+      </c>
+      <c r="I6">
+        <v>2.5027161182931814</v>
+      </c>
+      <c r="J6">
+        <v>5.4920410258454865E-2</v>
+      </c>
+      <c r="K6">
+        <v>4.9851984012279855</v>
+      </c>
+      <c r="L6">
+        <v>2.8011402713128071</v>
+      </c>
+      <c r="M6">
+        <v>4.2805027559879196</v>
+      </c>
+      <c r="N6">
+        <v>2.5879374445563008</v>
+      </c>
+      <c r="O6">
+        <v>9.6185473501649618E-2</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>100.00000000000003</v>
+      </c>
+      <c r="S6">
+        <v>203</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>2.5833634446121714E-2</v>
+      </c>
+      <c r="U6" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="V6" s="22">
+        <v>40.81</v>
+      </c>
+      <c r="W6" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="X6" s="22">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="Y6" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>49.49</v>
+      </c>
+      <c r="AA6" s="23">
+        <v>0.06</v>
+      </c>
+      <c r="AB6" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="AC6" s="24">
+        <v>1.06</v>
+      </c>
+      <c r="AD6" s="22">
+        <f t="shared" si="1"/>
+        <v>101.25</v>
+      </c>
+      <c r="AE6" s="26">
+        <f t="shared" si="2"/>
+        <v>90.167719492792259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1289.3781626256937</v>
+      </c>
+      <c r="B7">
+        <v>1109.7684914689307</v>
+      </c>
+      <c r="C7">
+        <v>179.60967115676294</v>
+      </c>
+      <c r="D7">
+        <v>6.9282240422985373</v>
+      </c>
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7">
+        <v>67.729723803163665</v>
+      </c>
+      <c r="G7">
+        <v>0.24200863177409873</v>
+      </c>
+      <c r="H7">
+        <v>14.719666689923949</v>
+      </c>
+      <c r="I7">
+        <v>2.5027161182931814</v>
+      </c>
+      <c r="J7">
+        <v>5.4920410258454865E-2</v>
+      </c>
+      <c r="K7">
+        <v>4.9851984012279855</v>
+      </c>
+      <c r="L7">
+        <v>2.8011402713128071</v>
+      </c>
+      <c r="M7">
+        <v>4.2805027559879196</v>
+      </c>
+      <c r="N7">
+        <v>2.5879374445563008</v>
+      </c>
+      <c r="O7">
+        <v>9.6185473501649618E-2</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>100.00000000000003</v>
+      </c>
+      <c r="S7">
+        <v>203</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>2.5833634446121714E-2</v>
+      </c>
+      <c r="U7" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="V7" s="22">
+        <v>39.409999999999997</v>
+      </c>
+      <c r="W7" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="X7" s="22">
+        <v>15.01</v>
+      </c>
+      <c r="Y7" s="23">
+        <v>0.24</v>
+      </c>
+      <c r="Z7" s="22">
+        <v>44.03</v>
+      </c>
+      <c r="AA7" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="AB7" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="AC7" s="24">
+        <v>1.21</v>
+      </c>
+      <c r="AD7" s="22">
+        <f t="shared" si="1"/>
+        <v>99.989999999999981</v>
+      </c>
+      <c r="AE7" s="26">
+        <f t="shared" si="2"/>
+        <v>83.946176526070587</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1289.4575135657428</v>
+      </c>
+      <c r="B8">
+        <v>1224.3543053647527</v>
+      </c>
+      <c r="C8">
+        <v>65.103208200990139</v>
+      </c>
+      <c r="D8">
+        <v>1.9956251781419221</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8">
+        <v>52.118830534583942</v>
+      </c>
+      <c r="G8">
+        <v>0.85819954385597064</v>
+      </c>
+      <c r="H8">
+        <v>14.107591787382404</v>
+      </c>
+      <c r="I8">
+        <v>8.3296771123685378</v>
+      </c>
+      <c r="J8">
+        <v>0.15309709666684737</v>
+      </c>
+      <c r="K8">
+        <v>12.18995979289525</v>
+      </c>
+      <c r="L8">
+        <v>8.3885775041149895</v>
+      </c>
+      <c r="M8">
+        <v>2.5319608675839991</v>
+      </c>
+      <c r="N8">
+        <v>1.1486733740974437</v>
+      </c>
+      <c r="O8">
+        <v>0.17343238645060602</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S8">
+        <v>314</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>3.9959414857547879E-2</v>
+      </c>
+      <c r="U8" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="V8" s="22">
+        <v>41.28</v>
+      </c>
+      <c r="W8" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X8" s="22">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="Z8" s="22">
+        <v>50.62</v>
+      </c>
+      <c r="AA8" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB8" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="AC8" s="24">
+        <v>0.48</v>
+      </c>
+      <c r="AD8" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE8" s="26">
+        <f t="shared" si="2"/>
+        <v>91.856289946628934</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1291.1142859217866</v>
+      </c>
+      <c r="B9">
+        <v>1241.1335739014639</v>
+      </c>
+      <c r="C9">
+        <v>49.980712020322699</v>
+      </c>
+      <c r="D9">
+        <v>1.4797897281806343</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9">
+        <v>52.118830534583942</v>
+      </c>
+      <c r="G9">
+        <v>0.85819954385597064</v>
+      </c>
+      <c r="H9">
+        <v>14.107591787382404</v>
+      </c>
+      <c r="I9">
+        <v>8.3296771123685378</v>
+      </c>
+      <c r="J9">
+        <v>0.15309709666684737</v>
+      </c>
+      <c r="K9">
+        <v>12.18995979289525</v>
+      </c>
+      <c r="L9">
+        <v>8.3885775041149895</v>
+      </c>
+      <c r="M9">
+        <v>2.5319608675839991</v>
+      </c>
+      <c r="N9">
+        <v>1.1486733740974437</v>
+      </c>
+      <c r="O9">
+        <v>0.17343238645060602</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S9">
+        <v>314</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>3.9959414857547879E-2</v>
+      </c>
+      <c r="U9" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="V9" s="22">
+        <v>41.6</v>
+      </c>
+      <c r="W9" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="X9" s="22">
+        <v>8.33</v>
+      </c>
+      <c r="Y9" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Z9" s="22">
+        <v>50.65</v>
+      </c>
+      <c r="AA9" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB9" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="AC9" s="24">
+        <v>0.45</v>
+      </c>
+      <c r="AD9" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE9" s="26">
+        <f t="shared" si="2"/>
+        <v>91.553334881009917</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1293.4050600585688</v>
+      </c>
+      <c r="B10">
+        <v>1245.2408988970028</v>
+      </c>
+      <c r="C10">
+        <v>48.164161161565971</v>
+      </c>
+      <c r="D10">
+        <v>1.4199547608602519</v>
+      </c>
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10">
+        <v>52.118830534583942</v>
+      </c>
+      <c r="G10">
+        <v>0.85819954385597064</v>
+      </c>
+      <c r="H10">
+        <v>14.107591787382404</v>
+      </c>
+      <c r="I10">
+        <v>8.3296771123685378</v>
+      </c>
+      <c r="J10">
+        <v>0.15309709666684737</v>
+      </c>
+      <c r="K10">
+        <v>12.18995979289525</v>
+      </c>
+      <c r="L10">
+        <v>8.3885775041149895</v>
+      </c>
+      <c r="M10">
+        <v>2.5319608675839991</v>
+      </c>
+      <c r="N10">
+        <v>1.1486733740974437</v>
+      </c>
+      <c r="O10">
+        <v>0.17343238645060602</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S10">
+        <v>314</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>3.9959414857547879E-2</v>
+      </c>
+      <c r="U10" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="V10" s="22">
+        <v>41.35</v>
+      </c>
+      <c r="W10" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X10" s="22">
+        <v>8.84</v>
+      </c>
+      <c r="Y10" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="Z10" s="22">
+        <v>50.05</v>
+      </c>
+      <c r="AA10" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="AB10" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="AC10" s="24">
+        <v>0.44</v>
+      </c>
+      <c r="AD10" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE10" s="26">
+        <f t="shared" si="2"/>
+        <v>90.985041403709872</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1280.0686969107805</v>
+      </c>
+      <c r="B11">
+        <v>1236.7817905790484</v>
+      </c>
+      <c r="C11">
+        <v>43.286906331732098</v>
+      </c>
+      <c r="D11">
+        <v>1.2615621948194937</v>
+      </c>
+      <c r="E11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11">
+        <v>52.196441509690892</v>
+      </c>
+      <c r="G11">
+        <v>0.78083955494990709</v>
+      </c>
+      <c r="H11">
+        <v>15.673697677703496</v>
+      </c>
+      <c r="I11">
+        <v>7.8393893111153803</v>
+      </c>
+      <c r="J11">
+        <v>0.14145349563902535</v>
+      </c>
+      <c r="K11">
+        <v>11.626115648394574</v>
+      </c>
+      <c r="L11">
+        <v>8.2167002517099945</v>
+      </c>
+      <c r="M11">
+        <v>2.3751383287147552</v>
+      </c>
+      <c r="N11">
+        <v>0.97564296812520268</v>
+      </c>
+      <c r="O11">
+        <v>0.17458125395678559</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>100.00000000000001</v>
+      </c>
+      <c r="S11">
+        <v>316</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>4.0213933423519518E-2</v>
+      </c>
+      <c r="U11" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="V11" s="22">
+        <v>41.01</v>
+      </c>
+      <c r="W11" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X11" s="22">
+        <v>9</v>
+      </c>
+      <c r="Y11" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="Z11" s="22">
+        <v>50.23</v>
+      </c>
+      <c r="AA11" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="AB11" s="23">
+        <v>0.08</v>
+      </c>
+      <c r="AC11" s="24">
+        <v>0.47</v>
+      </c>
+      <c r="AD11" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE11" s="26">
+        <f t="shared" si="2"/>
+        <v>90.866663300399679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1272.7028130559484</v>
+      </c>
+      <c r="B12">
+        <v>1267.7673433580708</v>
+      </c>
+      <c r="C12">
+        <v>4.9354696978775792</v>
+      </c>
+      <c r="D12">
+        <v>0.13074745938332147</v>
+      </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <v>52.196441509690892</v>
+      </c>
+      <c r="G12">
+        <v>0.78083955494990709</v>
+      </c>
+      <c r="H12">
+        <v>15.673697677703496</v>
+      </c>
+      <c r="I12">
+        <v>7.8393893111153803</v>
+      </c>
+      <c r="J12">
+        <v>0.14145349563902535</v>
+      </c>
+      <c r="K12">
+        <v>11.626115648394574</v>
+      </c>
+      <c r="L12">
+        <v>8.2167002517099945</v>
+      </c>
+      <c r="M12">
+        <v>2.3751383287147552</v>
+      </c>
+      <c r="N12">
+        <v>0.97564296812520268</v>
+      </c>
+      <c r="O12">
+        <v>0.17458125395678559</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>100.00000000000001</v>
+      </c>
+      <c r="S12">
+        <v>316</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>4.0213933423519518E-2</v>
+      </c>
+      <c r="U12" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="V12" s="22">
+        <v>41.53</v>
+      </c>
+      <c r="W12" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X12" s="22">
+        <v>7.28</v>
+      </c>
+      <c r="Y12" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="Z12" s="22">
+        <v>51.94</v>
+      </c>
+      <c r="AA12" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="AB12" s="23">
+        <v>0.08</v>
+      </c>
+      <c r="AC12" s="24">
+        <v>0.42</v>
+      </c>
+      <c r="AD12" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE12" s="26">
+        <f t="shared" si="2"/>
+        <v>92.710403936965093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1274.0829339471252</v>
+      </c>
+      <c r="B13">
+        <v>1259.6271105488831</v>
+      </c>
+      <c r="C13">
+        <v>14.455823398242046</v>
+      </c>
+      <c r="D13">
+        <v>0.3924745031543404</v>
+      </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <v>52.196441509690892</v>
+      </c>
+      <c r="G13">
+        <v>0.78083955494990709</v>
+      </c>
+      <c r="H13">
+        <v>15.673697677703496</v>
+      </c>
+      <c r="I13">
+        <v>7.8393893111153803</v>
+      </c>
+      <c r="J13">
+        <v>0.14145349563902535</v>
+      </c>
+      <c r="K13">
+        <v>11.626115648394574</v>
+      </c>
+      <c r="L13">
+        <v>8.2167002517099945</v>
+      </c>
+      <c r="M13">
+        <v>2.3751383287147552</v>
+      </c>
+      <c r="N13">
+        <v>0.97564296812520268</v>
+      </c>
+      <c r="O13">
+        <v>0.17458125395678559</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>100.00000000000001</v>
+      </c>
+      <c r="S13">
+        <v>316</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>4.0213933423519518E-2</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="V13" s="22">
+        <v>40.72</v>
+      </c>
+      <c r="W13" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X13" s="22">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="Y13" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="Z13" s="22">
+        <v>51.28</v>
+      </c>
+      <c r="AA13" s="23">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AB13" s="23">
+        <v>0.08</v>
+      </c>
+      <c r="AC13" s="24">
+        <v>0.43</v>
+      </c>
+      <c r="AD13" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE13" s="26">
+        <f t="shared" si="2"/>
+        <v>91.841806765783318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1259.6131314576905</v>
+      </c>
+      <c r="B14">
+        <v>1214.6437480369364</v>
+      </c>
+      <c r="C14">
+        <v>44.969383420754184</v>
+      </c>
+      <c r="D14">
+        <v>1.3158301161456116</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14">
+        <v>52.319115372855315</v>
+      </c>
+      <c r="G14">
+        <v>0.95083137312815591</v>
+      </c>
+      <c r="H14">
+        <v>14.960108316223266</v>
+      </c>
+      <c r="I14">
+        <v>7.7529255516187323</v>
+      </c>
+      <c r="J14">
+        <v>0.14289050590598884</v>
+      </c>
+      <c r="K14">
+        <v>10.784033404306101</v>
+      </c>
+      <c r="L14">
+        <v>8.4254081689353537</v>
+      </c>
+      <c r="M14">
+        <v>2.8727820314643173</v>
+      </c>
+      <c r="N14">
+        <v>1.5051196997935061</v>
+      </c>
+      <c r="O14">
+        <v>0.28678557576923946</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>99.999999999999972</v>
+      </c>
+      <c r="S14">
+        <v>243</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>3.0924005765554565E-2</v>
+      </c>
+      <c r="U14" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="V14" s="22">
+        <v>40.31</v>
+      </c>
+      <c r="W14" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X14" s="22">
+        <v>8.33</v>
+      </c>
+      <c r="Y14" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="Z14" s="22">
+        <v>51.2</v>
+      </c>
+      <c r="AA14" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="AB14" s="23">
+        <v>0.09</v>
+      </c>
+      <c r="AC14" s="24">
+        <v>0.41</v>
+      </c>
+      <c r="AD14" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE14" s="26">
+        <f t="shared" si="2"/>
+        <v>91.636481848035118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1267.8537702551648</v>
+      </c>
+      <c r="B15">
+        <v>1282.3409267688967</v>
+      </c>
+      <c r="C15">
+        <v>-14.487156513731861</v>
+      </c>
+      <c r="D15">
+        <v>-0.36432169218084715</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15">
+        <v>52.319115372855315</v>
+      </c>
+      <c r="G15">
+        <v>0.95083137312815591</v>
+      </c>
+      <c r="H15">
+        <v>14.960108316223266</v>
+      </c>
+      <c r="I15">
+        <v>7.7529255516187323</v>
+      </c>
+      <c r="J15">
+        <v>0.14289050590598884</v>
+      </c>
+      <c r="K15">
+        <v>10.784033404306101</v>
+      </c>
+      <c r="L15">
+        <v>8.4254081689353537</v>
+      </c>
+      <c r="M15">
+        <v>2.8727820314643173</v>
+      </c>
+      <c r="N15">
+        <v>1.5051196997935061</v>
+      </c>
+      <c r="O15">
+        <v>0.28678557576923946</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>99.999999999999972</v>
+      </c>
+      <c r="S15">
+        <v>243</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>3.0924005765554565E-2</v>
+      </c>
+      <c r="U15" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="V15" s="22">
+        <v>40.28</v>
+      </c>
+      <c r="W15" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X15" s="22">
+        <v>10.27</v>
+      </c>
+      <c r="Y15" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="Z15" s="22">
+        <v>49.81</v>
+      </c>
+      <c r="AA15" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="AB15" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="AC15" s="24">
+        <v>0.31</v>
+      </c>
+      <c r="AD15" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE15" s="26">
+        <f t="shared" si="2"/>
+        <v>89.63269420252864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1267.0372744250867</v>
+      </c>
+      <c r="B16">
+        <v>1274.3019044179314</v>
+      </c>
+      <c r="C16">
+        <v>-7.2646299928446751</v>
+      </c>
+      <c r="D16">
+        <v>-0.18631958523734798</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16">
+        <v>52.319115372855315</v>
+      </c>
+      <c r="G16">
+        <v>0.95083137312815591</v>
+      </c>
+      <c r="H16">
+        <v>14.960108316223266</v>
+      </c>
+      <c r="I16">
+        <v>7.7529255516187323</v>
+      </c>
+      <c r="J16">
+        <v>0.14289050590598884</v>
+      </c>
+      <c r="K16">
+        <v>10.784033404306101</v>
+      </c>
+      <c r="L16">
+        <v>8.4254081689353537</v>
+      </c>
+      <c r="M16">
+        <v>2.8727820314643173</v>
+      </c>
+      <c r="N16">
+        <v>1.5051196997935061</v>
+      </c>
+      <c r="O16">
+        <v>0.28678557576923946</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>99.999999999999972</v>
+      </c>
+      <c r="S16">
+        <v>243</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>3.0924005765554565E-2</v>
+      </c>
+      <c r="U16" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="V16" s="22">
+        <v>40.42</v>
+      </c>
+      <c r="W16" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X16" s="22">
+        <v>9.92</v>
+      </c>
+      <c r="Y16" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="Z16" s="22">
+        <v>49.94</v>
+      </c>
+      <c r="AA16" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="AB16" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC16" s="24">
+        <v>0.32</v>
+      </c>
+      <c r="AD16" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE16" s="26">
+        <f t="shared" si="2"/>
+        <v>89.974041157459638</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1264.2867189930939</v>
+      </c>
+      <c r="B17">
+        <v>1265.0333607995985</v>
+      </c>
+      <c r="C17">
+        <v>-0.74664180650461276</v>
+      </c>
+      <c r="D17">
+        <v>-1.9486122206925596E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17">
+        <v>51.331886132261687</v>
+      </c>
+      <c r="G17">
+        <v>0.62426424783180046</v>
+      </c>
+      <c r="H17">
+        <v>15.52354623270972</v>
+      </c>
+      <c r="I17">
+        <v>7.9033094358069054</v>
+      </c>
+      <c r="J17">
+        <v>0.13649592390901641</v>
+      </c>
+      <c r="K17">
+        <v>11.676338370021373</v>
+      </c>
+      <c r="L17">
+        <v>9.903001872768634</v>
+      </c>
+      <c r="M17">
+        <v>2.3138080896303799</v>
+      </c>
+      <c r="N17">
+        <v>0.49490232929129668</v>
+      </c>
+      <c r="O17">
+        <v>9.2447365769176781E-2</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S17">
+        <v>267</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>3.3978228557214274E-2</v>
+      </c>
+      <c r="U17" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="V17" s="22">
+        <v>41.24</v>
+      </c>
+      <c r="W17" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="X17" s="22">
+        <v>7.57</v>
+      </c>
+      <c r="Y17" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="Z17" s="22">
+        <v>51.49</v>
+      </c>
+      <c r="AA17" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="AB17" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="AC17" s="24">
+        <v>0.34</v>
+      </c>
+      <c r="AD17" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE17" s="26">
+        <f t="shared" si="2"/>
+        <v>92.380947662394405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1273.325049284957</v>
+      </c>
+      <c r="B18">
+        <v>1241.2644942018005</v>
+      </c>
+      <c r="C18">
+        <v>32.060555083156487</v>
+      </c>
+      <c r="D18">
+        <v>0.90948294703098287</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18">
+        <v>51.331886132261687</v>
+      </c>
+      <c r="G18">
+        <v>0.62426424783180046</v>
+      </c>
+      <c r="H18">
+        <v>15.52354623270972</v>
+      </c>
+      <c r="I18">
+        <v>7.9033094358069054</v>
+      </c>
+      <c r="J18">
+        <v>0.13649592390901641</v>
+      </c>
+      <c r="K18">
+        <v>11.676338370021373</v>
+      </c>
+      <c r="L18">
+        <v>9.903001872768634</v>
+      </c>
+      <c r="M18">
+        <v>2.3138080896303799</v>
+      </c>
+      <c r="N18">
+        <v>0.49490232929129668</v>
+      </c>
+      <c r="O18">
+        <v>9.2447365769176781E-2</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S18">
+        <v>267</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="0"/>
+        <v>3.3978228557214274E-2</v>
+      </c>
+      <c r="U18" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="V18" s="22">
+        <v>40.85</v>
+      </c>
+      <c r="W18" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="X18" s="22">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="Y18" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Z18" s="22">
+        <v>49.62</v>
+      </c>
+      <c r="AA18" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB18" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC18" s="24">
+        <v>0.37</v>
+      </c>
+      <c r="AD18" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE18" s="26">
+        <f t="shared" si="2"/>
+        <v>90.181757017795462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1265.2556502283128</v>
+      </c>
+      <c r="B19">
+        <v>1280.9238168882371</v>
+      </c>
+      <c r="C19">
+        <v>-15.668166659924282</v>
+      </c>
+      <c r="D19">
+        <v>-0.39274166931233312</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19">
+        <v>51.331886132261687</v>
+      </c>
+      <c r="G19">
+        <v>0.62426424783180046</v>
+      </c>
+      <c r="H19">
+        <v>15.52354623270972</v>
+      </c>
+      <c r="I19">
+        <v>7.9033094358069054</v>
+      </c>
+      <c r="J19">
+        <v>0.13649592390901641</v>
+      </c>
+      <c r="K19">
+        <v>11.676338370021373</v>
+      </c>
+      <c r="L19">
+        <v>9.903001872768634</v>
+      </c>
+      <c r="M19">
+        <v>2.3138080896303799</v>
+      </c>
+      <c r="N19">
+        <v>0.49490232929129668</v>
+      </c>
+      <c r="O19">
+        <v>9.2447365769176781E-2</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S19">
+        <v>267</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="0"/>
+        <v>3.3978228557214274E-2</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="V19" s="22">
+        <v>41.33</v>
+      </c>
+      <c r="W19" s="23">
+        <v>0.06</v>
+      </c>
+      <c r="X19" s="22">
+        <v>7.8</v>
+      </c>
+      <c r="Y19" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="Z19" s="22">
+        <v>51.45</v>
+      </c>
+      <c r="AA19" s="23">
+        <v>0.17</v>
+      </c>
+      <c r="AB19" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="AC19" s="24">
+        <v>0.32</v>
+      </c>
+      <c r="AD19" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE19" s="26">
+        <f t="shared" si="2"/>
+        <v>92.161976523717087</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1283.7075527572997</v>
+      </c>
+      <c r="B20">
+        <v>1181.8743032651869</v>
+      </c>
+      <c r="C20">
+        <v>101.83324949211283</v>
+      </c>
+      <c r="D20">
+        <v>3.3802434844952933</v>
+      </c>
+      <c r="E20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20">
+        <v>53.087041317611181</v>
+      </c>
+      <c r="G20">
+        <v>0.81523356744393027</v>
+      </c>
+      <c r="H20">
+        <v>14.268908020869176</v>
+      </c>
+      <c r="I20">
+        <v>8.1090516149797178</v>
+      </c>
+      <c r="J20">
+        <v>0.1452891506335717</v>
+      </c>
+      <c r="K20">
+        <v>11.974751974267681</v>
+      </c>
+      <c r="L20">
+        <v>7.9177542333121815</v>
+      </c>
+      <c r="M20">
+        <v>2.3308819152338711</v>
+      </c>
+      <c r="N20">
+        <v>1.1857209015595385</v>
+      </c>
+      <c r="O20">
+        <v>0.16536730408918335</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>100.00000000000004</v>
+      </c>
+      <c r="S20">
+        <v>281</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="0"/>
+        <v>3.5759858519015773E-2</v>
+      </c>
+      <c r="U20" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="V20" s="22">
+        <v>40.33</v>
+      </c>
+      <c r="W20" s="23">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="X20" s="22">
+        <v>8</v>
+      </c>
+      <c r="Y20" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="Z20" s="22">
+        <v>50.79</v>
+      </c>
+      <c r="AA20" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="AB20" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC20" s="24">
+        <v>0.53</v>
+      </c>
+      <c r="AD20" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE20" s="26">
+        <f t="shared" si="2"/>
+        <v>91.881334904619223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1288.2431115387622</v>
+      </c>
+      <c r="B21">
+        <v>1278.2783716576905</v>
+      </c>
+      <c r="C21">
+        <v>9.9647398810716368</v>
+      </c>
+      <c r="D21">
+        <v>0.26744635433493874</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21">
+        <v>53.087041317611181</v>
+      </c>
+      <c r="G21">
+        <v>0.81523356744393027</v>
+      </c>
+      <c r="H21">
+        <v>14.268908020869176</v>
+      </c>
+      <c r="I21">
+        <v>8.1090516149797178</v>
+      </c>
+      <c r="J21">
+        <v>0.1452891506335717</v>
+      </c>
+      <c r="K21">
+        <v>11.974751974267681</v>
+      </c>
+      <c r="L21">
+        <v>7.9177542333121815</v>
+      </c>
+      <c r="M21">
+        <v>2.3308819152338711</v>
+      </c>
+      <c r="N21">
+        <v>1.1857209015595385</v>
+      </c>
+      <c r="O21">
+        <v>0.16536730408918335</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>100.00000000000004</v>
+      </c>
+      <c r="S21">
+        <v>281</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="0"/>
+        <v>3.5759858519015773E-2</v>
+      </c>
+      <c r="U21" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="V21" s="22">
+        <v>39.909999999999997</v>
+      </c>
+      <c r="W21" s="23">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="X21" s="22">
+        <v>8.99</v>
+      </c>
+      <c r="Y21" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="Z21" s="22">
+        <v>49.52</v>
+      </c>
+      <c r="AA21" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="AB21" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC21" s="24">
+        <v>0.35</v>
+      </c>
+      <c r="AD21" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE21" s="26">
+        <f t="shared" si="2"/>
+        <v>90.757158568507521</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1290.836446054851</v>
+      </c>
+      <c r="B22">
+        <v>1279.0114690914756</v>
+      </c>
+      <c r="C22">
+        <v>11.82497696337532</v>
+      </c>
+      <c r="D22">
+        <v>0.31889533406869675</v>
+      </c>
+      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22">
+        <v>53.087041317611181</v>
+      </c>
+      <c r="G22">
+        <v>0.81523356744393027</v>
+      </c>
+      <c r="H22">
+        <v>14.268908020869176</v>
+      </c>
+      <c r="I22">
+        <v>8.1090516149797178</v>
+      </c>
+      <c r="J22">
+        <v>0.1452891506335717</v>
+      </c>
+      <c r="K22">
+        <v>11.974751974267681</v>
+      </c>
+      <c r="L22">
+        <v>7.9177542333121815</v>
+      </c>
+      <c r="M22">
+        <v>2.3308819152338711</v>
+      </c>
+      <c r="N22">
+        <v>1.1857209015595385</v>
+      </c>
+      <c r="O22">
+        <v>0.16536730408918335</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>100.00000000000004</v>
+      </c>
+      <c r="S22">
+        <v>281</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>3.5759858519015773E-2</v>
+      </c>
+      <c r="U22" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="V22" s="22">
+        <v>40.18</v>
+      </c>
+      <c r="W22" s="23">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="X22" s="22">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="Y22" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Z22" s="22">
+        <v>49.31</v>
+      </c>
+      <c r="AA22" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="AB22" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC22" s="24">
+        <v>0.35</v>
+      </c>
+      <c r="AD22" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE22" s="26">
+        <f t="shared" si="2"/>
+        <v>90.274223318339651</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1250.909850062294</v>
+      </c>
+      <c r="B23">
+        <v>1266.8142644073037</v>
+      </c>
+      <c r="C23">
+        <v>-15.904414345009627</v>
+      </c>
+      <c r="D23">
+        <v>-0.39840360330395969</v>
+      </c>
+      <c r="E23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23">
+        <v>54.577101078531456</v>
+      </c>
+      <c r="G23">
+        <v>0.73516060959420904</v>
+      </c>
+      <c r="H23">
+        <v>14.883471797996261</v>
+      </c>
+      <c r="I23">
+        <v>7.0581672631608674</v>
+      </c>
+      <c r="J23">
+        <v>0.13214330386504033</v>
+      </c>
+      <c r="K23">
+        <v>10.177858834637281</v>
+      </c>
+      <c r="L23">
+        <v>8.0388521487913422</v>
+      </c>
+      <c r="M23">
+        <v>2.7272965699229736</v>
+      </c>
+      <c r="N23">
+        <v>1.4776849300144854</v>
+      </c>
+      <c r="O23">
+        <v>0.19226346348608156</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S23">
+        <v>246</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="0"/>
+        <v>3.1305783614512028E-2</v>
+      </c>
+      <c r="U23" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="V23" s="22">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="W23" s="23">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="X23" s="22">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Y23" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="Z23" s="22">
+        <v>51.16</v>
+      </c>
+      <c r="AA23" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="AB23" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC23" s="24">
+        <v>0.36</v>
+      </c>
+      <c r="AD23" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE23" s="26">
+        <f t="shared" si="2"/>
+        <v>91.750331197096003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1258.4431329385311</v>
+      </c>
+      <c r="B24">
+        <v>1264.3133450370115</v>
+      </c>
+      <c r="C24">
+        <v>-5.8702120984803514</v>
+      </c>
+      <c r="D24">
+        <v>-0.15112245590395831</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24">
+        <v>54.577101078531456</v>
+      </c>
+      <c r="G24">
+        <v>0.73516060959420904</v>
+      </c>
+      <c r="H24">
+        <v>14.883471797996261</v>
+      </c>
+      <c r="I24">
+        <v>7.0581672631608674</v>
+      </c>
+      <c r="J24">
+        <v>0.13214330386504033</v>
+      </c>
+      <c r="K24">
+        <v>10.177858834637281</v>
+      </c>
+      <c r="L24">
+        <v>8.0388521487913422</v>
+      </c>
+      <c r="M24">
+        <v>2.7272965699229736</v>
+      </c>
+      <c r="N24">
+        <v>1.4776849300144854</v>
+      </c>
+      <c r="O24">
+        <v>0.19226346348608156</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S24">
+        <v>246</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>3.1305783614512028E-2</v>
+      </c>
+      <c r="U24" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="V24" s="22">
+        <v>40.44</v>
+      </c>
+      <c r="W24" s="23">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="X24" s="22">
+        <v>9.68</v>
+      </c>
+      <c r="Y24" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="Z24" s="22">
+        <v>49.57</v>
+      </c>
+      <c r="AA24" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB24" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC24" s="24">
+        <v>0.36</v>
+      </c>
+      <c r="AD24" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE24" s="26">
+        <f t="shared" si="2"/>
+        <v>90.126840742101493</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>1250.1236203880139</v>
+      </c>
+      <c r="B25">
+        <v>1254.1058793546222</v>
+      </c>
+      <c r="C25">
+        <v>-3.9822589666082422</v>
+      </c>
+      <c r="D25">
+        <v>-0.10303913152579586</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25">
+        <v>54.577101078531456</v>
+      </c>
+      <c r="G25">
+        <v>0.73516060959420904</v>
+      </c>
+      <c r="H25">
+        <v>14.883471797996261</v>
+      </c>
+      <c r="I25">
+        <v>7.0581672631608674</v>
+      </c>
+      <c r="J25">
+        <v>0.13214330386504033</v>
+      </c>
+      <c r="K25">
+        <v>10.177858834637281</v>
+      </c>
+      <c r="L25">
+        <v>8.0388521487913422</v>
+      </c>
+      <c r="M25">
+        <v>2.7272965699229736</v>
+      </c>
+      <c r="N25">
+        <v>1.4776849300144854</v>
+      </c>
+      <c r="O25">
+        <v>0.19226346348608156</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S25">
+        <v>246</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>3.1305783614512028E-2</v>
+      </c>
+      <c r="U25" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="V25" s="22">
+        <v>40.9</v>
+      </c>
+      <c r="W25" s="23">
+        <v>5.8700000000000002E-2</v>
+      </c>
+      <c r="X25" s="22">
+        <v>7.93</v>
+      </c>
+      <c r="Y25" s="23">
+        <v>0.12</v>
+      </c>
+      <c r="Z25" s="22">
+        <v>51.44</v>
+      </c>
+      <c r="AA25" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="AB25" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC25" s="24">
+        <v>0.38</v>
+      </c>
+      <c r="AD25" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE25" s="26">
+        <f t="shared" si="2"/>
+        <v>92.040315020017488</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>1263.8956125973618</v>
+      </c>
+      <c r="B26">
+        <v>1196.4274035939175</v>
+      </c>
+      <c r="C26">
+        <v>67.468209003444372</v>
+      </c>
+      <c r="D26">
+        <v>2.079157237070878</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26">
+        <v>54.348233103220416</v>
+      </c>
+      <c r="G26">
+        <v>0.74120055867879475</v>
+      </c>
+      <c r="H26">
+        <v>14.933344012975768</v>
+      </c>
+      <c r="I26">
+        <v>7.2063557222024768</v>
+      </c>
+      <c r="J26">
+        <v>0.13386264311138033</v>
+      </c>
+      <c r="K26">
+        <v>10.236737636228018</v>
+      </c>
+      <c r="L26">
+        <v>7.9952141852350609</v>
+      </c>
+      <c r="M26">
+        <v>2.7762731719038629</v>
+      </c>
+      <c r="N26">
+        <v>1.4315393202741329</v>
+      </c>
+      <c r="O26">
+        <v>0.19723964617009668</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S26">
+        <v>252.39999999999998</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>3.2120243025621283E-2</v>
+      </c>
+      <c r="U26" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="V26" s="22">
+        <v>39.5</v>
+      </c>
+      <c r="W26" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="X26" s="22">
+        <v>10.99</v>
+      </c>
+      <c r="Y26" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Z26" s="22">
+        <v>48.26</v>
+      </c>
+      <c r="AA26" s="23">
+        <v>0.09</v>
+      </c>
+      <c r="AB26" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="AC26" s="24">
+        <v>0.48</v>
+      </c>
+      <c r="AD26" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE26" s="26">
+        <f t="shared" si="2"/>
+        <v>88.672249910115241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>1260.8434272019676</v>
+      </c>
+      <c r="B27">
+        <v>1269.3125179422195</v>
+      </c>
+      <c r="C27">
+        <v>-8.469090740251886</v>
+      </c>
+      <c r="D27">
+        <v>-0.21650539843773772</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27">
+        <v>54.348233103220416</v>
+      </c>
+      <c r="G27">
+        <v>0.74120055867879475</v>
+      </c>
+      <c r="H27">
+        <v>14.933344012975768</v>
+      </c>
+      <c r="I27">
+        <v>7.2063557222024768</v>
+      </c>
+      <c r="J27">
+        <v>0.13386264311138033</v>
+      </c>
+      <c r="K27">
+        <v>10.236737636228018</v>
+      </c>
+      <c r="L27">
+        <v>7.9952141852350609</v>
+      </c>
+      <c r="M27">
+        <v>2.7762731719038629</v>
+      </c>
+      <c r="N27">
+        <v>1.4315393202741329</v>
+      </c>
+      <c r="O27">
+        <v>0.19723964617009668</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S27">
+        <v>252.39999999999998</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="0"/>
+        <v>3.2120243025621283E-2</v>
+      </c>
+      <c r="U27" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="V27" s="22">
+        <v>40.380000000000003</v>
+      </c>
+      <c r="W27" s="23">
+        <v>0</v>
+      </c>
+      <c r="X27" s="22">
+        <v>10.38</v>
+      </c>
+      <c r="Y27" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="Z27" s="22">
+        <v>49.42</v>
+      </c>
+      <c r="AA27" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="AB27" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="24">
+        <v>0.36</v>
+      </c>
+      <c r="AD27" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE27" s="26">
+        <f t="shared" si="2"/>
+        <v>89.459382263601682</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>1234.534618366175</v>
+      </c>
+      <c r="B28">
+        <v>1255.8900658209877</v>
+      </c>
+      <c r="C28">
+        <v>-21.355447454812747</v>
+      </c>
+      <c r="D28">
+        <v>-0.52689916113142465</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28">
+        <v>54.348233103220416</v>
+      </c>
+      <c r="G28">
+        <v>0.74120055867879475</v>
+      </c>
+      <c r="H28">
+        <v>14.933344012975768</v>
+      </c>
+      <c r="I28">
+        <v>7.2063557222024768</v>
+      </c>
+      <c r="J28">
+        <v>0.13386264311138033</v>
+      </c>
+      <c r="K28">
+        <v>10.236737636228018</v>
+      </c>
+      <c r="L28">
+        <v>7.9952141852350609</v>
+      </c>
+      <c r="M28">
+        <v>2.7762731719038629</v>
+      </c>
+      <c r="N28">
+        <v>1.4315393202741329</v>
+      </c>
+      <c r="O28">
+        <v>0.19723964617009668</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>99.999999999999986</v>
+      </c>
+      <c r="S28">
+        <v>252.39999999999998</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>3.2120243025621283E-2</v>
+      </c>
+      <c r="U28" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="V28" s="22">
+        <v>37.4</v>
+      </c>
+      <c r="W28" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="X28" s="22">
+        <v>7</v>
+      </c>
+      <c r="Y28" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="Z28" s="22">
+        <v>53.36</v>
+      </c>
+      <c r="AA28" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="AB28" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="AC28" s="24">
+        <v>0.38</v>
+      </c>
+      <c r="AD28" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE28" s="26">
+        <f t="shared" si="2"/>
+        <v>93.14529604931063</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>1217.7011885407123</v>
+      </c>
+      <c r="B29">
+        <v>1254.5415364058845</v>
+      </c>
+      <c r="C29">
+        <v>-36.840347865172134</v>
+      </c>
+      <c r="D29">
+        <v>-0.86949543862672418</v>
+      </c>
+      <c r="E29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29">
+        <v>56.06103503331417</v>
+      </c>
+      <c r="G29">
+        <v>0.98080428917691143</v>
+      </c>
+      <c r="H29">
+        <v>15.569632041702326</v>
+      </c>
+      <c r="I29">
+        <v>6.6067306821338345</v>
+      </c>
+      <c r="J29">
+        <v>0.11690125382418294</v>
+      </c>
+      <c r="K29">
+        <v>7.7580944444632829</v>
+      </c>
+      <c r="L29">
+        <v>6.9354045989114779</v>
+      </c>
+      <c r="M29">
+        <v>3.6342870493522414</v>
+      </c>
+      <c r="N29">
+        <v>2.0574884680125147</v>
+      </c>
+      <c r="O29">
+        <v>0.2796221391090411</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>99.999999999999957</v>
+      </c>
+      <c r="S29">
+        <v>165</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>2.0997781692660509E-2</v>
+      </c>
+      <c r="U29" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="V29" s="22">
+        <v>39.57</v>
+      </c>
+      <c r="W29" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="X29" s="22">
+        <v>11.51</v>
+      </c>
+      <c r="Y29" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="Z29" s="22">
+        <v>48.49</v>
+      </c>
+      <c r="AA29" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB29" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="AC29" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AD29" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE29" s="26">
+        <f t="shared" si="2"/>
+        <v>88.248912551002519</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>1215.325202539143</v>
+      </c>
+      <c r="B30">
+        <v>1273.1401437940426</v>
+      </c>
+      <c r="C30">
+        <v>-57.814941254899622</v>
+      </c>
+      <c r="D30">
+        <v>-1.2806519819554834</v>
+      </c>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30">
+        <v>56.06103503331417</v>
+      </c>
+      <c r="G30">
+        <v>0.98080428917691143</v>
+      </c>
+      <c r="H30">
+        <v>15.569632041702326</v>
+      </c>
+      <c r="I30">
+        <v>6.6067306821338345</v>
+      </c>
+      <c r="J30">
+        <v>0.11690125382418294</v>
+      </c>
+      <c r="K30">
+        <v>7.7580944444632829</v>
+      </c>
+      <c r="L30">
+        <v>6.9354045989114779</v>
+      </c>
+      <c r="M30">
+        <v>3.6342870493522414</v>
+      </c>
+      <c r="N30">
+        <v>2.0574884680125147</v>
+      </c>
+      <c r="O30">
+        <v>0.2796221391090411</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <v>99.999999999999957</v>
+      </c>
+      <c r="S30">
+        <v>165</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>2.0997781692660509E-2</v>
+      </c>
+      <c r="U30" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="V30" s="22">
+        <v>39.65</v>
+      </c>
+      <c r="W30" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="X30" s="22">
+        <v>10.96</v>
+      </c>
+      <c r="Y30" s="23">
+        <v>0.16</v>
+      </c>
+      <c r="Z30" s="22">
+        <v>48.97</v>
+      </c>
+      <c r="AA30" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="AB30" s="23">
+        <v>0.04</v>
+      </c>
+      <c r="AC30" s="24">
+        <v>0.27</v>
+      </c>
+      <c r="AD30" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE30" s="26">
+        <f t="shared" si="2"/>
+        <v>88.845241357057645</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>1218.1797246752394</v>
+      </c>
+      <c r="B31">
+        <v>1254.6944849070933</v>
+      </c>
+      <c r="C31">
+        <v>-36.51476023185387</v>
+      </c>
+      <c r="D31">
+        <v>-0.86263336870325502</v>
+      </c>
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31">
+        <v>56.06103503331417</v>
+      </c>
+      <c r="G31">
+        <v>0.98080428917691143</v>
+      </c>
+      <c r="H31">
+        <v>15.569632041702326</v>
+      </c>
+      <c r="I31">
+        <v>6.6067306821338345</v>
+      </c>
+      <c r="J31">
+        <v>0.11690125382418294</v>
+      </c>
+      <c r="K31">
+        <v>7.7580944444632829</v>
+      </c>
+      <c r="L31">
+        <v>6.9354045989114779</v>
+      </c>
+      <c r="M31">
+        <v>3.6342870493522414</v>
+      </c>
+      <c r="N31">
+        <v>2.0574884680125147</v>
+      </c>
+      <c r="O31">
+        <v>0.2796221391090411</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>99.999999999999957</v>
+      </c>
+      <c r="S31">
+        <v>165</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="0"/>
+        <v>2.0997781692660509E-2</v>
+      </c>
+      <c r="U31" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="V31" s="22">
+        <v>39.68</v>
+      </c>
+      <c r="W31" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="X31" s="22">
+        <v>11.56</v>
+      </c>
+      <c r="Y31" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="Z31" s="22">
+        <v>48.45</v>
+      </c>
+      <c r="AA31" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AB31" s="23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC31" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AD31" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE31" s="26">
+        <f t="shared" si="2"/>
+        <v>88.195297694572844</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>1276.2305116754083</v>
+      </c>
+      <c r="B32">
+        <v>1430.5443666847182</v>
+      </c>
+      <c r="C32">
+        <v>-154.31385500930992</v>
+      </c>
+      <c r="D32">
+        <v>-2.3881544820329061</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32">
+        <v>57.739169568186405</v>
+      </c>
+      <c r="G32">
+        <v>0.62292538713589107</v>
+      </c>
+      <c r="H32">
+        <v>14.477121741106336</v>
+      </c>
+      <c r="I32">
+        <v>5.6179076897714024</v>
+      </c>
+      <c r="J32">
+        <v>9.8003411779909594E-2</v>
+      </c>
+      <c r="K32">
+        <v>9.8635173954035054</v>
+      </c>
+      <c r="L32">
+        <v>6.5765657878299066</v>
+      </c>
+      <c r="M32">
+        <v>2.7829705760919574</v>
+      </c>
+      <c r="N32">
+        <v>2.114039400310022</v>
+      </c>
+      <c r="O32">
+        <v>0.10777904238469567</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>100.00000000000003</v>
+      </c>
+      <c r="S32">
+        <v>320</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="0"/>
+        <v>4.0722970555462798E-2</v>
+      </c>
+      <c r="U32" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="V32" s="22">
+        <v>40.98</v>
+      </c>
+      <c r="W32" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="X32" s="22">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="Y32" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Z32" s="22">
+        <v>49.47</v>
+      </c>
+      <c r="AA32" s="23">
+        <v>0.24</v>
+      </c>
+      <c r="AB32" s="23">
+        <v>0.09</v>
+      </c>
+      <c r="AC32" s="24">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AD32" s="22">
+        <v>100.0458</v>
+      </c>
+      <c r="AE32" s="26">
+        <f t="shared" si="2"/>
+        <v>90.478665786320533</v>
+      </c>
+    </row>
+    <row r="33" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U33" s="23"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="22"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="23"/>
+      <c r="AB33" s="23"/>
+      <c r="AC33" s="24"/>
+      <c r="AD33" s="22"/>
+      <c r="AE33" s="26"/>
+    </row>
+    <row r="34" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U34" s="23"/>
+      <c r="V34" s="22"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="22"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="22"/>
+      <c r="AA34" s="23"/>
+      <c r="AB34" s="23"/>
+      <c r="AC34" s="24"/>
+      <c r="AD34" s="22"/>
+      <c r="AE34" s="26"/>
+    </row>
+    <row r="35" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U35" s="23"/>
+      <c r="V35" s="22"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="22"/>
+      <c r="Y35" s="23"/>
+      <c r="Z35" s="22"/>
+      <c r="AA35" s="23"/>
+      <c r="AB35" s="23"/>
+      <c r="AC35" s="24"/>
+      <c r="AD35" s="22"/>
+      <c r="AE35" s="26"/>
+    </row>
+    <row r="36" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U36" s="23"/>
+      <c r="V36" s="22"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="22"/>
+      <c r="AA36" s="23"/>
+      <c r="AB36" s="23"/>
+      <c r="AC36" s="24"/>
+      <c r="AD36" s="22"/>
+      <c r="AE36" s="26"/>
+    </row>
+    <row r="37" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U37" s="23"/>
+      <c r="V37" s="22"/>
+      <c r="W37" s="23"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="23"/>
+      <c r="Z37" s="22"/>
+      <c r="AA37" s="23"/>
+      <c r="AB37" s="23"/>
+      <c r="AC37" s="24"/>
+      <c r="AD37" s="22"/>
+      <c r="AE37" s="26"/>
+    </row>
+    <row r="38" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U38" s="23"/>
+      <c r="V38" s="22"/>
+      <c r="W38" s="23"/>
+      <c r="X38" s="22"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="22"/>
+      <c r="AA38" s="23"/>
+      <c r="AB38" s="23"/>
+      <c r="AC38" s="24"/>
+      <c r="AD38" s="22"/>
+      <c r="AE38" s="26"/>
+    </row>
+    <row r="39" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U39" s="23"/>
+      <c r="V39" s="22"/>
+      <c r="W39" s="23"/>
+      <c r="X39" s="22"/>
+      <c r="Y39" s="23"/>
+      <c r="Z39" s="22"/>
+      <c r="AA39" s="23"/>
+      <c r="AB39" s="23"/>
+      <c r="AC39" s="24"/>
+      <c r="AD39" s="22"/>
+      <c r="AE39" s="26"/>
+    </row>
+    <row r="40" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U40" s="23"/>
+      <c r="V40" s="22"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="22"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="22"/>
+      <c r="AA40" s="23"/>
+      <c r="AB40" s="23"/>
+      <c r="AC40" s="24"/>
+      <c r="AD40" s="22"/>
+      <c r="AE40" s="26"/>
+    </row>
+    <row r="41" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U41" s="23"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="23"/>
+      <c r="X41" s="22"/>
+      <c r="Y41" s="23"/>
+      <c r="Z41" s="22"/>
+      <c r="AA41" s="23"/>
+      <c r="AB41" s="23"/>
+      <c r="AC41" s="24"/>
+      <c r="AD41" s="22"/>
+      <c r="AE41" s="26"/>
+    </row>
+    <row r="42" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U42" s="23"/>
+      <c r="V42" s="22"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="22"/>
+      <c r="Y42" s="23"/>
+      <c r="Z42" s="22"/>
+      <c r="AA42" s="23"/>
+      <c r="AB42" s="23"/>
+      <c r="AC42" s="24"/>
+      <c r="AD42" s="22"/>
+      <c r="AE42" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAFB0FCC-31C5-A347-849A-21A9BAF70A22}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
@@ -3017,19 +6468,19 @@
       <selection sqref="A1:AB1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.296875" customWidth="1"/>
-    <col min="18" max="18" width="49.296875" customWidth="1"/>
-    <col min="29" max="33" width="11.19921875" style="6"/>
-    <col min="34" max="34" width="11.19921875" style="16" customWidth="1"/>
-    <col min="35" max="35" width="11.19921875" style="6"/>
-    <col min="36" max="37" width="11.19921875" style="6" customWidth="1"/>
-    <col min="43" max="43" width="11.19921875" style="20"/>
-    <col min="44" max="44" width="11.19921875" style="6"/>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="18" max="18" width="49.33203125" customWidth="1"/>
+    <col min="29" max="33" width="11.1640625" style="6"/>
+    <col min="34" max="34" width="11.1640625" style="16" customWidth="1"/>
+    <col min="35" max="35" width="11.1640625" style="6"/>
+    <col min="36" max="37" width="11.1640625" style="6" customWidth="1"/>
+    <col min="43" max="43" width="11.1640625" style="20"/>
+    <col min="44" max="44" width="11.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="13" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="13" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -3169,7 +6620,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3307,7 +6758,7 @@
         <v>1021.4977612489276</v>
       </c>
     </row>
-    <row r="3" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3445,7 +6896,7 @@
         <v>969.30470589090635</v>
       </c>
     </row>
-    <row r="4" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -3583,7 +7034,7 @@
         <v>1008.3926959575062</v>
       </c>
     </row>
-    <row r="5" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3721,7 +7172,7 @@
         <v>932.4066154671109</v>
       </c>
     </row>
-    <row r="6" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -3859,7 +7310,7 @@
         <v>994.52289560698819</v>
       </c>
     </row>
-    <row r="7" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -3997,7 +7448,7 @@
         <v>980.5957950395333</v>
       </c>
     </row>
-    <row r="8" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -4135,7 +7586,7 @@
         <v>970.95243031259167</v>
       </c>
     </row>
-    <row r="9" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -4273,7 +7724,7 @@
         <v>938.81426399564441</v>
       </c>
     </row>
-    <row r="10" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -4411,7 +7862,7 @@
         <v>908.55665230590898</v>
       </c>
     </row>
-    <row r="11" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -4549,7 +8000,7 @@
         <v>1046.213289112063</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.35">
       <c r="P12" s="1"/>
     </row>
   </sheetData>
@@ -4559,7 +8010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2758E642-A654-4573-9A36-AD6F514C2950}">
   <dimension ref="A1:AP14"/>
   <sheetViews>
@@ -4567,29 +8018,29 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.296875" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875"/>
-    <col min="4" max="4" width="11.19921875"/>
-    <col min="6" max="6" width="11.19921875"/>
-    <col min="8" max="8" width="11.19921875"/>
-    <col min="10" max="10" width="11.19921875"/>
-    <col min="12" max="12" width="11.19921875"/>
-    <col min="14" max="14" width="11.19921875"/>
-    <col min="16" max="16" width="11.19921875"/>
-    <col min="18" max="18" width="11.19921875"/>
-    <col min="20" max="21" width="11.19921875" customWidth="1"/>
-    <col min="22" max="22" width="11.19921875"/>
-    <col min="24" max="24" width="11.19921875"/>
-    <col min="26" max="27" width="11.19921875"/>
-    <col min="29" max="29" width="11.19921875"/>
-    <col min="31" max="31" width="11.19921875"/>
-    <col min="32" max="32" width="49.296875" customWidth="1"/>
-    <col min="33" max="42" width="11.19921875"/>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625"/>
+    <col min="4" max="4" width="11.1640625"/>
+    <col min="6" max="6" width="11.1640625"/>
+    <col min="8" max="8" width="11.1640625"/>
+    <col min="10" max="10" width="11.1640625"/>
+    <col min="12" max="12" width="11.1640625"/>
+    <col min="14" max="14" width="11.1640625"/>
+    <col min="16" max="16" width="11.1640625"/>
+    <col min="18" max="18" width="11.1640625"/>
+    <col min="20" max="21" width="11.1640625" customWidth="1"/>
+    <col min="22" max="22" width="11.1640625"/>
+    <col min="24" max="24" width="11.1640625"/>
+    <col min="26" max="27" width="11.1640625"/>
+    <col min="29" max="29" width="11.1640625"/>
+    <col min="31" max="31" width="11.1640625"/>
+    <col min="32" max="32" width="49.33203125" customWidth="1"/>
+    <col min="33" max="42" width="11.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -4717,7 +8168,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -4845,7 +8296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -4973,7 +8424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -5101,7 +8552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -5229,7 +8680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -5357,7 +8808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -5485,7 +8936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -5613,7 +9064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -5741,7 +9192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -5869,7 +9320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -5997,12 +9448,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
       <c r="Y12" s="2"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -6039,7 +9490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE45F4C-AD22-4802-854F-449443DEFF24}">
   <dimension ref="A1:AP14"/>
   <sheetViews>
@@ -6047,14 +9498,14 @@
       <selection activeCell="W14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.296875" customWidth="1"/>
-    <col min="20" max="21" width="11.19921875" customWidth="1"/>
-    <col min="32" max="32" width="49.296875" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="20" max="21" width="11.1640625" customWidth="1"/>
+    <col min="32" max="32" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -6182,7 +9633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -6310,7 +9761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -6438,7 +9889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -6566,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -6694,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -6822,7 +10273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -6950,7 +10401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -7078,7 +10529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -7206,7 +10657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -7334,7 +10785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -7462,12 +10913,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
       <c r="Y12" s="2"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>

</xml_diff>